<commit_message>
Update Skills Cert3 widget.
</commit_message>
<xml_diff>
--- a/dashboard_loader/education_participation_uploader/education_participation.xlsx
+++ b/dashboard_loader/education_participation_uploader/education_participation.xlsx
@@ -280,7 +280,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -632,7 +632,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>